<commit_message>
burndown is klaar en product backlog aangepast weer
</commit_message>
<xml_diff>
--- a/documentatie/Excel bestanden/Product backlog overview & Sprint backlogs(2).xlsx
+++ b/documentatie/Excel bestanden/Product backlog overview & Sprint backlogs(2).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6336" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>Er is een ERD en een RRM van het database.</t>
   </si>
   <si>
-    <t>Als user wil ik een ERD en een RRM van het database zien</t>
-  </si>
-  <si>
     <t>1. Maak een ERD 2. Maak een RRM</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>1. Het moet kunnen werken als je ze hebt gekoppeld aan elkaar</t>
+  </si>
+  <si>
+    <t>Als user wil ik een ERD en een RM van het database zien</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1494,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -1510,7 +1510,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>8</v>
@@ -39561,7 +39561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -39689,7 +39689,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>8</v>
@@ -39698,10 +39698,10 @@
         <v>12</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="9" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
@@ -39709,7 +39709,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>8</v>
@@ -39718,10 +39718,10 @@
         <v>12</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
@@ -39797,8 +39797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -39845,7 +39845,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C3" s="46" t="s">
         <v>8</v>
@@ -39854,10 +39854,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="9" customFormat="1" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>